<commit_message>
made a better previous and next song method
</commit_message>
<xml_diff>
--- a/songsV2.xlsx
+++ b/songsV2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frcprogramming/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frcprogramming/git/FinalProjectCS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0552F518-38A7-FC49-BB77-1EC75785C625}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2B71B9-2A9A-2E4B-AFA7-CB5AAF3A76B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{AFBE1522-0DB0-864C-B0E6-D890F6E73F64}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" xr2:uid="{AFBE1522-0DB0-864C-B0E6-D890F6E73F64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BF2DAD-D4C9-AA41-B909-45A54E08B08F}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>